<commit_message>
Adds 1va to excel
</commit_message>
<xml_diff>
--- a/src/rahul/analysis_log.xlsx
+++ b/src/rahul/analysis_log.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\univ_work\454_FinalProject\src\rahul\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rahul/GDrive NU/454 Adv Modeling/454_FinalProject/src/rahul/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11916" xr2:uid="{22B8B965-45EB-4B97-A737-B8527EF79BBB}"/>
+    <workbookView xWindow="2780" yWindow="460" windowWidth="25600" windowHeight="11920"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>data</t>
   </si>
@@ -84,12 +90,15 @@
   </si>
   <si>
     <t>/xgb_trad_004</t>
+  </si>
+  <si>
+    <t>max 1vA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,9 +135,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,26 +452,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31BC230B-8F77-4B8F-879C-ECB65E03E4F7}">
-  <dimension ref="A1:K6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="14.21875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="1"/>
-    <col min="8" max="8" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="5" width="14.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="1"/>
+    <col min="8" max="8" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,7 +506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -531,7 +541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -566,7 +576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -601,7 +611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -636,7 +646,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -669,6 +679,41 @@
       </c>
       <c r="K6" s="1">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>120</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.92859999999999998</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.88480000000000003</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>